<commit_message>
Update component BOM values
- Change C1 tolerance to 20%
- Change all resistors to 1% tolerance
- Change F1 to handle increased LED current (previous part unsuitable)
- Ensure all supplier part numbers are correct
</commit_message>
<xml_diff>
--- a/Source/Outputs/irprobe_v150_BOM.xlsx
+++ b/Source/Outputs/irprobe_v150_BOM.xlsx
@@ -3,9 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F9537D72-9233-415F-A941-415809CF3D68}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Git\z-probe\Source\Outputs\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D543D433-0552-4F14-A82F-F47CFA78966B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2280" yWindow="0" windowWidth="21600" windowHeight="12735" xr2:uid="{88A72022-FA9F-454F-A370-96E24896E228}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{8437657F-6CD3-4F59-9EB0-983859B725D9}"/>
   </bookViews>
   <sheets>
     <sheet name="irprobe_v150_BOM" sheetId="1" r:id="rId1"/>
@@ -26,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="110">
   <si>
     <t>Designator</t>
   </si>
@@ -61,240 +66,246 @@
     <t>Capacitor, Ceramic (SMD)</t>
   </si>
   <si>
-    <t>22uF 10% 16V X7R 1210</t>
+    <t>22uF 20% 16V X7R 1210</t>
   </si>
   <si>
     <t>Approved Sub OK</t>
   </si>
   <si>
+    <t>TDK</t>
+  </si>
+  <si>
+    <t>C3225X7R1C226M250AC</t>
+  </si>
+  <si>
+    <t>Digi-Key</t>
+  </si>
+  <si>
+    <t>445-3955-1-ND</t>
+  </si>
+  <si>
+    <t>C2</t>
+  </si>
+  <si>
+    <t>100nF 10% 50V X7R 0603</t>
+  </si>
+  <si>
+    <t>Yageo</t>
+  </si>
+  <si>
+    <t>CC0603KRX7R9BB104</t>
+  </si>
+  <si>
+    <t>311-1344-1-ND</t>
+  </si>
+  <si>
+    <t>C3</t>
+  </si>
+  <si>
+    <t>1nF 10% 50V X7R 0603</t>
+  </si>
+  <si>
+    <t>CC0603KRX7R9BB102</t>
+  </si>
+  <si>
+    <t>311-1080-1-ND</t>
+  </si>
+  <si>
+    <t>P1</t>
+  </si>
+  <si>
+    <t>Connector (SMD)</t>
+  </si>
+  <si>
+    <t>JST-SH 4P Side-Entry .1"</t>
+  </si>
+  <si>
+    <t>JST</t>
+  </si>
+  <si>
+    <t>SM04B-SRSS-TB(LF)(SN)</t>
+  </si>
+  <si>
+    <t>455-1804-1-ND</t>
+  </si>
+  <si>
+    <t>D2</t>
+  </si>
+  <si>
+    <t>Diode, Schottky (SMD)</t>
+  </si>
+  <si>
+    <t>Dual 100mA 30V SOT523</t>
+  </si>
+  <si>
+    <t>MCC</t>
+  </si>
+  <si>
+    <t>BAT54ST-TP</t>
+  </si>
+  <si>
+    <t>BAT54ST-TPCT-ND</t>
+  </si>
+  <si>
+    <t>D1</t>
+  </si>
+  <si>
+    <t>Diode, Zener (SMD)</t>
+  </si>
+  <si>
+    <t>5.6V 0.5W SOD-123</t>
+  </si>
+  <si>
+    <t>Diodes</t>
+  </si>
+  <si>
+    <t>BZT52C5V6-7-F</t>
+  </si>
+  <si>
+    <t>BZT52C5V6-FDICT-ND</t>
+  </si>
+  <si>
+    <t>L1</t>
+  </si>
+  <si>
+    <t>Inductor (SMD)</t>
+  </si>
+  <si>
+    <t>1uH 20% 600mA 0603</t>
+  </si>
+  <si>
+    <t>MLZ1608A1R0WT000</t>
+  </si>
+  <si>
+    <t>445-6384-1-ND</t>
+  </si>
+  <si>
+    <t>LD1, LD2</t>
+  </si>
+  <si>
+    <t>LED (SMD)</t>
+  </si>
+  <si>
+    <t>IR 950nm 1.6V 70mA Side-View</t>
+  </si>
+  <si>
+    <t>Osram Opto</t>
+  </si>
+  <si>
+    <t>SFH4045N</t>
+  </si>
+  <si>
+    <t>475-3047-1-ND</t>
+  </si>
+  <si>
+    <t>LD3</t>
+  </si>
+  <si>
+    <t>Red 0603</t>
+  </si>
+  <si>
+    <t>Vishay Lite-On</t>
+  </si>
+  <si>
+    <t>LTST-C190KRKT</t>
+  </si>
+  <si>
+    <t>160-1436-1-ND</t>
+  </si>
+  <si>
+    <t>LD4, LD5</t>
+  </si>
+  <si>
+    <t>White Side-View 0602</t>
+  </si>
+  <si>
+    <t>QT-Brightek</t>
+  </si>
+  <si>
+    <t>QBLP617-IW</t>
+  </si>
+  <si>
+    <t>1516-1080-1-ND</t>
+  </si>
+  <si>
+    <t>U1</t>
+  </si>
+  <si>
+    <t>Microcontroller (SMD)</t>
+  </si>
+  <si>
+    <t>ATtiny44A-MU - 8-bit AVR Microcontroller,  20MHz, 1.8-5.5V, 4KB Flash, 256 Bytes EEPROM, 256 Bytes SRAM, 20-pin MLF, Industrial Grade (-40°C to 85°C), Pb-Free</t>
+  </si>
+  <si>
+    <t>Microchip / Atmel</t>
+  </si>
+  <si>
+    <t>ATTINY44A-MU</t>
+  </si>
+  <si>
+    <t>ATTINY44A-MU-ND</t>
+  </si>
+  <si>
+    <t>Q2</t>
+  </si>
+  <si>
+    <t>MOSFET (SMD)</t>
+  </si>
+  <si>
+    <t>N-CH MOSFET 30V 5.7A SOT23</t>
+  </si>
+  <si>
+    <t>Alpha &amp; Omega Semiconductor</t>
+  </si>
+  <si>
+    <t>AO3400A</t>
+  </si>
+  <si>
+    <t>785-1000-1-ND</t>
+  </si>
+  <si>
+    <t>Q1</t>
+  </si>
+  <si>
+    <t>Phototransistor (SMD)</t>
+  </si>
+  <si>
+    <t>NPN 30V 15mA IR 870nm Side-View</t>
+  </si>
+  <si>
+    <t>SFH3015FA</t>
+  </si>
+  <si>
+    <t>475-2914-1-ND</t>
+  </si>
+  <si>
+    <t>F1</t>
+  </si>
+  <si>
+    <t>PTC Resettable Fuse (SMD)</t>
+  </si>
+  <si>
+    <t>60V 200mA Hold 400mA Trip 1206</t>
+  </si>
+  <si>
+    <t>Bel</t>
+  </si>
+  <si>
+    <t>0ZCJ0020FF2E</t>
+  </si>
+  <si>
+    <t>507-1797-1-ND</t>
+  </si>
+  <si>
+    <t>F2</t>
+  </si>
+  <si>
+    <t>24V 14mA Hold 29mA Trip 220R 0603</t>
+  </si>
+  <si>
     <t>Murata</t>
   </si>
   <si>
-    <t>GRM32ER71C226MEA8L</t>
-  </si>
-  <si>
-    <t>Digi-Key</t>
-  </si>
-  <si>
-    <t>490-5956-1-ND</t>
-  </si>
-  <si>
-    <t>C2</t>
-  </si>
-  <si>
-    <t>100nF 10% 50V X7R 0603</t>
-  </si>
-  <si>
-    <t>Yageo</t>
-  </si>
-  <si>
-    <t>CC0603KRX7R9BB104</t>
-  </si>
-  <si>
-    <t>311-1344-1-ND</t>
-  </si>
-  <si>
-    <t>C3</t>
-  </si>
-  <si>
-    <t>1nF 10% 50V X7R 0603</t>
-  </si>
-  <si>
-    <t>P1</t>
-  </si>
-  <si>
-    <t>Connector (SMD)</t>
-  </si>
-  <si>
-    <t>JST-SH 4P Side-Entry .1"</t>
-  </si>
-  <si>
-    <t>JST</t>
-  </si>
-  <si>
-    <t>SM04B-SRSS-TB(LF)(SN)</t>
-  </si>
-  <si>
-    <t>455-1804-1-ND</t>
-  </si>
-  <si>
-    <t>D2</t>
-  </si>
-  <si>
-    <t>Diode, Schottky (SMD)</t>
-  </si>
-  <si>
-    <t>Dual 100mA 30V SOT523</t>
-  </si>
-  <si>
-    <t>MCC</t>
-  </si>
-  <si>
-    <t>BAT54ST-TP</t>
-  </si>
-  <si>
-    <t>BAT54ST-TPCT-ND</t>
-  </si>
-  <si>
-    <t>D1</t>
-  </si>
-  <si>
-    <t>Diode, Zener (SMD)</t>
-  </si>
-  <si>
-    <t>5.6V 0.5W SOD-123</t>
-  </si>
-  <si>
-    <t>Diodes</t>
-  </si>
-  <si>
-    <t>BZT52C5V6-7-F</t>
-  </si>
-  <si>
-    <t>BZT52C5V6-FDICT-ND</t>
-  </si>
-  <si>
-    <t>L1</t>
-  </si>
-  <si>
-    <t>Inductor (SMD)</t>
-  </si>
-  <si>
-    <t>1uH 20% 600mA 0603</t>
-  </si>
-  <si>
-    <t>TDK</t>
-  </si>
-  <si>
-    <t>MLZ1608A1R0M</t>
-  </si>
-  <si>
-    <t>445-3163-2-ND</t>
-  </si>
-  <si>
-    <t>LD1, LD2</t>
-  </si>
-  <si>
-    <t>LED (SMD)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IR 950nm 1.6V 70mA Side-View </t>
-  </si>
-  <si>
-    <t>Osram Opto</t>
-  </si>
-  <si>
-    <t>SFH4045N</t>
-  </si>
-  <si>
-    <t>475-3047-1-ND</t>
-  </si>
-  <si>
-    <t>LD3</t>
-  </si>
-  <si>
-    <t>Red 0603</t>
-  </si>
-  <si>
-    <t>Vishay Lite-On</t>
-  </si>
-  <si>
-    <t>LTST-C190KGKT</t>
-  </si>
-  <si>
-    <t>160-1435-2-ND</t>
-  </si>
-  <si>
-    <t>LD4, LD5</t>
-  </si>
-  <si>
-    <t>White Side-View 0602</t>
-  </si>
-  <si>
-    <t>QT-Brightek</t>
-  </si>
-  <si>
-    <t>QBLP617-IW</t>
-  </si>
-  <si>
-    <t>1516-1080-1-ND</t>
-  </si>
-  <si>
-    <t>U1</t>
-  </si>
-  <si>
-    <t>Microcontroller (SMD)</t>
-  </si>
-  <si>
-    <t>ATtiny44A-MU - 8-bit AVR Microcontroller,  20MHz, 1.8-5.5V, 4KB Flash, 256 Bytes EEPROM, 256 Bytes SRAM, 20-pin MLF, Industrial Grade (-40°C to 85°C), Pb-Free</t>
-  </si>
-  <si>
-    <t>Microchip / Atmel</t>
-  </si>
-  <si>
-    <t>ATTINY44A-MU</t>
-  </si>
-  <si>
-    <t>ATTINY44A-MU-ND</t>
-  </si>
-  <si>
-    <t>Q2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MOSFET (SMD) </t>
-  </si>
-  <si>
-    <t>N-CH MOSFET 30V 5.7A SOT23</t>
-  </si>
-  <si>
-    <t>Alpha &amp; Omega Semiconductor</t>
-  </si>
-  <si>
-    <t>AO3400A</t>
-  </si>
-  <si>
-    <t>785-1000-1-ND</t>
-  </si>
-  <si>
-    <t>Q1</t>
-  </si>
-  <si>
-    <t>Phototransistor (SMD)</t>
-  </si>
-  <si>
-    <t>NPN 30V 15mA IR 870nm Side-View</t>
-  </si>
-  <si>
-    <t>SFH3015FA</t>
-  </si>
-  <si>
-    <t>475-2914-1-ND</t>
-  </si>
-  <si>
-    <t>F1</t>
-  </si>
-  <si>
-    <t>PTC Resettable Fuse (SMD)</t>
-  </si>
-  <si>
-    <t>60V 50mA Hold 150mA Trip 1206</t>
-  </si>
-  <si>
-    <t>Bel</t>
-  </si>
-  <si>
-    <t>0ZCJ0005FF2E</t>
-  </si>
-  <si>
-    <t>507-1793-1-ND</t>
-  </si>
-  <si>
-    <t>F2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">24V 14mA Hold 29mA Trip 220R 0603 </t>
-  </si>
-  <si>
     <t>PRG18BB221MB1RB</t>
   </si>
   <si>
@@ -307,25 +318,31 @@
     <t>Resistor (SMD)</t>
   </si>
   <si>
-    <t>330R 5% 100mW 0603</t>
-  </si>
-  <si>
-    <t>RC0603FR-071KL</t>
-  </si>
-  <si>
-    <t>311-1.00KHRCT-ND</t>
+    <t>330R 1% 100mW 0603</t>
+  </si>
+  <si>
+    <t>RC0603FR-07330RL</t>
+  </si>
+  <si>
+    <t>311-330HRCT-ND</t>
   </si>
   <si>
     <t>R2, R9</t>
   </si>
   <si>
-    <t>6K8 5% 100mW 0603</t>
+    <t>6K8 1% 100mW 0603</t>
+  </si>
+  <si>
+    <t>RC0603FR-076K8L</t>
+  </si>
+  <si>
+    <t>311-6.80KHRCT-ND</t>
   </si>
   <si>
     <t>R4, R7</t>
   </si>
   <si>
-    <t>100R 5% 100mW 0603</t>
+    <t>100R 1% 100mW 0603</t>
   </si>
   <si>
     <t>RC0603FR-07100RL</t>
@@ -337,7 +354,13 @@
     <t>R5</t>
   </si>
   <si>
-    <t>390R 5% 100mW 0603</t>
+    <t>390R 1% 100mW 0603</t>
+  </si>
+  <si>
+    <t>RC0603FR-07390RL</t>
+  </si>
+  <si>
+    <t>311-390HRCT-ND</t>
   </si>
 </sst>
 </file>
@@ -731,7 +754,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1219431-09D6-4045-868E-77CBC1D386BA}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EC7EED5-BD35-4B4A-953A-EC6A3226184B}">
   <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -746,7 +769,7 @@
     <col min="6" max="6" width="21" customWidth="1"/>
     <col min="7" max="7" width="13.5703125" customWidth="1"/>
     <col min="8" max="8" width="8.85546875" customWidth="1"/>
-    <col min="9" max="9" width="8.140625" customWidth="1"/>
+    <col min="9" max="9" width="18.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -856,24 +879,24 @@
         <v>19</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>15</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D5" s="3">
         <v>1</v>
@@ -882,27 +905,27 @@
         <v>12</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="H5" s="2" t="s">
         <v>15</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D6" s="3">
         <v>1</v>
@@ -911,27 +934,27 @@
         <v>12</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>15</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D7" s="3">
         <v>1</v>
@@ -940,27 +963,27 @@
         <v>12</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>15</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D8" s="3">
         <v>1</v>
@@ -969,27 +992,27 @@
         <v>12</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>45</v>
+        <v>13</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H8" s="2" t="s">
         <v>15</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D9" s="3">
         <v>2</v>
@@ -998,27 +1021,27 @@
         <v>12</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>15</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D10" s="3">
         <v>1</v>
@@ -1027,27 +1050,27 @@
         <v>12</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="H10" s="2" t="s">
         <v>15</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D11" s="3">
         <v>2</v>
@@ -1056,27 +1079,27 @@
         <v>12</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H11" s="2" t="s">
         <v>15</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D12" s="3">
         <v>1</v>
@@ -1085,27 +1108,27 @@
         <v>12</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="H12" s="2" t="s">
         <v>15</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D13" s="3">
         <v>1</v>
@@ -1114,27 +1137,27 @@
         <v>12</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="H13" s="2" t="s">
         <v>15</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D14" s="3">
         <v>1</v>
@@ -1143,27 +1166,27 @@
         <v>12</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="H14" s="2" t="s">
         <v>15</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D15" s="3">
         <v>1</v>
@@ -1172,27 +1195,27 @@
         <v>12</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H15" s="2" t="s">
         <v>15</v>
       </c>
       <c r="I15" s="4" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D16" s="3">
         <v>1</v>
@@ -1201,27 +1224,27 @@
         <v>12</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>13</v>
+        <v>90</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="H16" s="2" t="s">
         <v>15</v>
       </c>
       <c r="I16" s="4" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D17" s="3">
         <v>3</v>
@@ -1233,24 +1256,24 @@
         <v>19</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="H17" s="2" t="s">
         <v>15</v>
       </c>
       <c r="I17" s="4" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="D18" s="3">
         <v>2</v>
@@ -1262,24 +1285,24 @@
         <v>19</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="H18" s="2" t="s">
         <v>15</v>
       </c>
       <c r="I18" s="4" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="D19" s="3">
         <v>2</v>
@@ -1291,24 +1314,24 @@
         <v>19</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="H19" s="2" t="s">
         <v>15</v>
       </c>
       <c r="I19" s="4" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="D20" s="3">
         <v>1</v>
@@ -1320,74 +1343,74 @@
         <v>19</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>94</v>
+        <v>108</v>
       </c>
       <c r="H20" s="2" t="s">
         <v>15</v>
       </c>
       <c r="I20" s="4" t="s">
-        <v>95</v>
+        <v>109</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" tooltip="Component" display="'Murata" xr:uid="{A609B614-BEDE-401A-8A6E-CE05D1E6B4BB}"/>
-    <hyperlink ref="G2" r:id="rId2" tooltip="Manufacturer" display="'GRM32ER71C226MEA8L" xr:uid="{06002F2E-A2E1-4F77-8DFA-3B9DFD0BCDAC}"/>
-    <hyperlink ref="I2" r:id="rId3" tooltip="Supplier" display="'490-5956-1-ND" xr:uid="{14F302E4-6BAC-485D-88F7-4E2410447101}"/>
-    <hyperlink ref="F3" r:id="rId4" tooltip="Component" display="'Yageo" xr:uid="{9BD76A1E-D9DE-40DC-A14F-12291591779C}"/>
-    <hyperlink ref="G3" r:id="rId5" tooltip="Manufacturer" display="'CC0603KRX7R9BB104" xr:uid="{C3BAA2EF-F942-4AF2-93EB-ECDC34FE05B8}"/>
-    <hyperlink ref="I3" r:id="rId6" tooltip="Supplier" display="'311-1344-1-ND" xr:uid="{1CE01919-4242-4B07-936D-F12B35743568}"/>
-    <hyperlink ref="F4" r:id="rId7" tooltip="Component" display="'Yageo" xr:uid="{8F262DB8-5CC8-4B47-BECE-2D4F1F70E7A8}"/>
-    <hyperlink ref="G4" r:id="rId8" tooltip="Manufacturer" display="'CC0603KRX7R9BB104" xr:uid="{0FA3C1CB-8971-4DB7-8E56-1AF0613AE105}"/>
-    <hyperlink ref="I4" r:id="rId9" tooltip="Supplier" display="'311-1344-1-ND" xr:uid="{26285EE9-632A-412A-8778-8158DEEBFCAF}"/>
-    <hyperlink ref="F5" r:id="rId10" tooltip="Component" display="'JST" xr:uid="{6AF84B80-C29A-41E1-BFA4-D47E91CA529F}"/>
-    <hyperlink ref="G5" r:id="rId11" tooltip="Manufacturer" display="'SM04B-SRSS-TB(LF)(SN)" xr:uid="{F7B874C0-2D48-48C8-90E6-DD53AA2C42B7}"/>
-    <hyperlink ref="I5" r:id="rId12" tooltip="Supplier" display="'455-1804-1-ND" xr:uid="{9C8FD6AE-6A3C-4320-A8DB-FB5D64CAA729}"/>
-    <hyperlink ref="F6" r:id="rId13" tooltip="Component" display="'MCC" xr:uid="{6A9203B2-D2F2-43E0-8450-643C50B415F2}"/>
-    <hyperlink ref="G6" r:id="rId14" tooltip="Manufacturer" display="'BAT54ST-TP" xr:uid="{3C3C7083-3B20-4C59-A78E-C07BB400994C}"/>
-    <hyperlink ref="I6" r:id="rId15" tooltip="Supplier" display="'BAT54ST-TPCT-ND" xr:uid="{C55E98E9-4C64-4BB8-BF34-8E1649453220}"/>
-    <hyperlink ref="F7" r:id="rId16" tooltip="Component" display="'Diodes" xr:uid="{EE4B93BB-1761-4F0E-B44C-9CABC0E56129}"/>
-    <hyperlink ref="G7" r:id="rId17" tooltip="Manufacturer" display="'BZT52C5V6-7-F" xr:uid="{5A553F54-1C8F-47E2-90D3-10E135B85912}"/>
-    <hyperlink ref="I7" r:id="rId18" tooltip="Supplier" display="'BZT52C5V6-FDICT-ND" xr:uid="{269560AA-FB86-47CB-A33A-A6464B3052CC}"/>
-    <hyperlink ref="F8" r:id="rId19" tooltip="Component" display="'TDK" xr:uid="{825E4587-DE51-4049-A21A-471131A96F63}"/>
-    <hyperlink ref="G8" r:id="rId20" tooltip="Manufacturer" display="'MLZ1608A1R0M" xr:uid="{A7200CA9-EDD0-4F6C-9AEF-D9877B1FA145}"/>
-    <hyperlink ref="I8" r:id="rId21" tooltip="Supplier" display="'445-3163-2-ND" xr:uid="{EB6F3641-F70D-4091-BADE-785ADFBAA9C6}"/>
-    <hyperlink ref="F9" r:id="rId22" tooltip="Component" display="'Osram Opto" xr:uid="{7B18CDEA-B95F-43F3-B5F7-5D49175CD39D}"/>
-    <hyperlink ref="G9" r:id="rId23" tooltip="Manufacturer" display="'SFH4045N" xr:uid="{1E8F0EDB-BF13-4554-A54E-6312CC556725}"/>
-    <hyperlink ref="I9" r:id="rId24" tooltip="Supplier" display="'475-3047-1-ND" xr:uid="{EB63058B-42F9-43CB-ABDA-4E433E1E417F}"/>
-    <hyperlink ref="F10" r:id="rId25" tooltip="Component" display="'Vishay Lite-On" xr:uid="{25E5162B-3416-4AEB-8707-E7822A6478DC}"/>
-    <hyperlink ref="G10" r:id="rId26" tooltip="Manufacturer" display="'LTST-C190KGKT" xr:uid="{D4F25386-A5E8-4B45-B0D3-4865FF7B1B88}"/>
-    <hyperlink ref="I10" r:id="rId27" tooltip="Supplier" display="'160-1435-2-ND" xr:uid="{2F5F56BC-2AB2-4CE1-B297-C042305009B8}"/>
-    <hyperlink ref="F11" r:id="rId28" tooltip="Component" display="'QT-Brightek" xr:uid="{103277BE-548A-4D09-A55A-633582BA3412}"/>
-    <hyperlink ref="G11" r:id="rId29" tooltip="Manufacturer" display="'QBLP617-IW" xr:uid="{B6250F97-F03D-454C-9545-D1D81F4694A1}"/>
-    <hyperlink ref="I11" r:id="rId30" tooltip="Supplier" display="'1516-1080-1-ND" xr:uid="{E8A225DB-3047-4051-AC3D-B1B7EF90E161}"/>
-    <hyperlink ref="F12" r:id="rId31" tooltip="Component" display="'Microchip / Atmel" xr:uid="{76BBFA54-CF8F-424C-9F39-E4FEF6762C9E}"/>
-    <hyperlink ref="G12" r:id="rId32" tooltip="Manufacturer" display="'ATTINY44A-MU" xr:uid="{AE5EF29F-6A26-45E3-8AD3-2DCC24892B9B}"/>
-    <hyperlink ref="I12" r:id="rId33" tooltip="Supplier" display="'ATTINY44A-MU-ND" xr:uid="{99C6CDB9-7C54-4EC1-8B3C-6A059ED5E685}"/>
-    <hyperlink ref="F13" r:id="rId34" tooltip="Component" display="'Alpha &amp; Omega Semiconductor" xr:uid="{C07866D6-5C3E-432C-9FD9-659B0C22AD7B}"/>
-    <hyperlink ref="G13" r:id="rId35" tooltip="Manufacturer" display="'AO3400A" xr:uid="{1179B94E-A617-4176-A328-D6146CE6E675}"/>
-    <hyperlink ref="I13" r:id="rId36" tooltip="Supplier" display="'785-1000-1-ND" xr:uid="{BF148E28-A18E-4F6C-B30C-6D3D01CB0161}"/>
-    <hyperlink ref="F14" r:id="rId37" tooltip="Component" display="'Osram Opto" xr:uid="{E1DB03DA-64B0-43A1-9C2D-875713823A8D}"/>
-    <hyperlink ref="G14" r:id="rId38" tooltip="Manufacturer" display="'SFH3015FA" xr:uid="{B0B54820-9EF2-49A1-8C22-1D5297DF908C}"/>
-    <hyperlink ref="I14" r:id="rId39" tooltip="Supplier" display="'475-2914-1-ND" xr:uid="{0F89CEAA-77B4-45CC-98FF-27A2B6396A00}"/>
-    <hyperlink ref="F15" r:id="rId40" tooltip="Component" display="'Bel" xr:uid="{F5E679D8-EC2A-4115-9100-EDE3268A6EFF}"/>
-    <hyperlink ref="G15" r:id="rId41" tooltip="Manufacturer" display="'0ZCJ0005FF2E" xr:uid="{3BA0AB3A-65AA-403C-9BE2-1E2FD2099106}"/>
-    <hyperlink ref="I15" r:id="rId42" tooltip="Supplier" display="'507-1793-1-ND" xr:uid="{3B816811-B284-48FE-814B-0510CF3FE0D3}"/>
-    <hyperlink ref="F16" r:id="rId43" tooltip="Component" display="'Murata" xr:uid="{E3AE925B-9F65-4A3B-87DF-6E85DB318606}"/>
-    <hyperlink ref="G16" r:id="rId44" tooltip="Manufacturer" display="'PRG18BB221MB1RB" xr:uid="{DB1F5CAC-F802-42B6-A675-6ED9EAA3AB97}"/>
-    <hyperlink ref="I16" r:id="rId45" tooltip="Supplier" display="'490-2470-1-ND" xr:uid="{8A5A3223-02D6-4531-B642-8D02C6679EE9}"/>
-    <hyperlink ref="F17" r:id="rId46" tooltip="Component" display="'Yageo" xr:uid="{F8802BE7-D7B2-4FCC-9CCC-9DFB43C25E32}"/>
-    <hyperlink ref="G17" r:id="rId47" tooltip="Manufacturer" display="'RC0603FR-071KL" xr:uid="{C47FFAFC-0392-433B-AB42-E2B994665718}"/>
-    <hyperlink ref="I17" r:id="rId48" tooltip="Supplier" display="'311-1.00KHRCT-ND" xr:uid="{154DF78B-63DE-48D3-9BE4-9794D0ADB646}"/>
-    <hyperlink ref="F18" r:id="rId49" tooltip="Component" display="'Yageo" xr:uid="{30B74840-1EA1-4DB9-89DC-00064A688692}"/>
-    <hyperlink ref="G18" r:id="rId50" tooltip="Manufacturer" display="'RC0603FR-071KL" xr:uid="{2B0A472A-39FA-4377-82E9-D364C474F3D4}"/>
-    <hyperlink ref="I18" r:id="rId51" tooltip="Supplier" display="'311-1.00KHRCT-ND" xr:uid="{9A53CD62-EC8E-4E8A-8C6A-B5AD93C859D9}"/>
-    <hyperlink ref="F19" r:id="rId52" tooltip="Component" display="'Yageo" xr:uid="{99D796F9-E786-436E-8148-E6E952F1C994}"/>
-    <hyperlink ref="G19" r:id="rId53" tooltip="Manufacturer" display="'RC0603FR-07100RL" xr:uid="{4050362F-703D-4E51-AC4C-7230F33A0EBD}"/>
-    <hyperlink ref="I19" r:id="rId54" tooltip="Supplier" display="'311-100HRCT-ND" xr:uid="{6053DCB6-F752-4DD7-A56C-6BB781A07D84}"/>
-    <hyperlink ref="F20" r:id="rId55" tooltip="Component" display="'Yageo" xr:uid="{3306AEE5-557D-4088-B8E4-8D9420EAC58B}"/>
-    <hyperlink ref="G20" r:id="rId56" tooltip="Manufacturer" display="'RC0603FR-071KL" xr:uid="{192BA8C5-4A71-47AD-BBA5-4DE4CA3E67D9}"/>
-    <hyperlink ref="I20" r:id="rId57" tooltip="Supplier" display="'311-1.00KHRCT-ND" xr:uid="{4A95FB87-51F9-4071-B151-03359451D9D9}"/>
+    <hyperlink ref="F2" r:id="rId1" tooltip="Component" display="'TDK" xr:uid="{C96CC31C-1CFC-4602-8899-6C14DD1400FF}"/>
+    <hyperlink ref="G2" r:id="rId2" tooltip="Manufacturer" display="'C3225X7R1C226M250AC" xr:uid="{79C0FDFB-F5DB-476A-9F94-9AA2974F4F07}"/>
+    <hyperlink ref="I2" r:id="rId3" tooltip="Supplier" display="'445-3955-1-ND" xr:uid="{64C74F5E-A79C-4B81-A47E-B24C9AA6B6FB}"/>
+    <hyperlink ref="F3" r:id="rId4" tooltip="Component" display="'Yageo" xr:uid="{279B6E5C-CBCF-4787-B7FB-8761EAABEDFD}"/>
+    <hyperlink ref="G3" r:id="rId5" tooltip="Manufacturer" display="'CC0603KRX7R9BB104" xr:uid="{679A411C-FFD7-4AEC-9DAB-557803C6A0B5}"/>
+    <hyperlink ref="I3" r:id="rId6" tooltip="Supplier" display="'311-1344-1-ND" xr:uid="{DCE7FB78-1F69-4280-8F04-7B33813DEDEA}"/>
+    <hyperlink ref="F4" r:id="rId7" tooltip="Component" display="'Yageo" xr:uid="{18576A0F-65D3-42FB-B03C-191B38F80968}"/>
+    <hyperlink ref="G4" r:id="rId8" tooltip="Manufacturer" display="'CC0603KRX7R9BB102" xr:uid="{E4357864-F58F-49E8-9178-B7DFDCC2E862}"/>
+    <hyperlink ref="I4" r:id="rId9" tooltip="Supplier" display="'311-1080-1-ND" xr:uid="{1A1D8655-1E9C-414E-BCBC-B33BA8B69A30}"/>
+    <hyperlink ref="F5" r:id="rId10" tooltip="Component" display="'JST" xr:uid="{A7C72156-8BF6-4A2E-8E92-74F6A14DDEE1}"/>
+    <hyperlink ref="G5" r:id="rId11" tooltip="Manufacturer" display="'SM04B-SRSS-TB(LF)(SN)" xr:uid="{59166C2D-1352-4F5E-BC9D-9B6FB4FB952D}"/>
+    <hyperlink ref="I5" r:id="rId12" tooltip="Supplier" display="'455-1804-1-ND" xr:uid="{9F2B7AAD-8CAB-4EF2-8A0E-954A39DF54F8}"/>
+    <hyperlink ref="F6" r:id="rId13" tooltip="Component" display="'MCC" xr:uid="{2F525F87-47BF-4A8E-8875-340663F885F8}"/>
+    <hyperlink ref="G6" r:id="rId14" tooltip="Manufacturer" display="'BAT54ST-TP" xr:uid="{90A5BE59-A4D8-452D-AB03-73E3C3385DA0}"/>
+    <hyperlink ref="I6" r:id="rId15" tooltip="Supplier" display="'BAT54ST-TPCT-ND" xr:uid="{5B3454F3-F17A-46D3-A026-9C7DD9360821}"/>
+    <hyperlink ref="F7" r:id="rId16" tooltip="Component" display="'Diodes" xr:uid="{D8931F9A-977E-4CB5-AAED-823172718F3E}"/>
+    <hyperlink ref="G7" r:id="rId17" tooltip="Manufacturer" display="'BZT52C5V6-7-F" xr:uid="{71BC0F1A-CACE-41CC-95D6-8CAC6520BEBB}"/>
+    <hyperlink ref="I7" r:id="rId18" tooltip="Supplier" display="'BZT52C5V6-FDICT-ND" xr:uid="{591300F4-541F-49CB-BB05-56048A651F43}"/>
+    <hyperlink ref="F8" r:id="rId19" tooltip="Component" display="'TDK" xr:uid="{EF3DA59B-2A7F-48EA-ACBF-86221B0F5500}"/>
+    <hyperlink ref="G8" r:id="rId20" tooltip="Manufacturer" display="'MLZ1608A1R0WT000" xr:uid="{FB2164F2-4601-4874-AB4E-BC8D27D2FF7D}"/>
+    <hyperlink ref="I8" r:id="rId21" tooltip="Supplier" display="'445-6384-1-ND" xr:uid="{B4D77423-A4F9-4D71-B79B-06444CAAECC5}"/>
+    <hyperlink ref="F9" r:id="rId22" tooltip="Component" display="'Osram Opto" xr:uid="{234B9FC3-F770-4668-ADF5-A752FB0130D2}"/>
+    <hyperlink ref="G9" r:id="rId23" tooltip="Manufacturer" display="'SFH4045N" xr:uid="{21B46038-E6BF-46DE-B920-A294DF52D6CF}"/>
+    <hyperlink ref="I9" r:id="rId24" tooltip="Supplier" display="'475-3047-1-ND" xr:uid="{D224009A-1AD1-4F05-AB55-64C462082A9D}"/>
+    <hyperlink ref="F10" r:id="rId25" tooltip="Component" display="'Vishay Lite-On" xr:uid="{2787E8DE-54BD-42D7-8D79-41C7DCDC244A}"/>
+    <hyperlink ref="G10" r:id="rId26" tooltip="Manufacturer" display="'LTST-C190KRKT" xr:uid="{D0A8EDED-2DD8-480C-A64D-5858A9FD57BF}"/>
+    <hyperlink ref="I10" r:id="rId27" tooltip="Supplier" display="'160-1436-1-ND" xr:uid="{035CD29E-1DAE-4078-A978-55F885597662}"/>
+    <hyperlink ref="F11" r:id="rId28" tooltip="Component" display="'QT-Brightek" xr:uid="{E0E1D278-D54A-4ED3-A18A-8B5F2CBB35F8}"/>
+    <hyperlink ref="G11" r:id="rId29" tooltip="Manufacturer" display="'QBLP617-IW" xr:uid="{60AFBECB-10F3-4781-A764-D84B9184F18A}"/>
+    <hyperlink ref="I11" r:id="rId30" tooltip="Supplier" display="'1516-1080-1-ND" xr:uid="{507FDEE1-DFEE-49A2-937C-04E318CE4C8B}"/>
+    <hyperlink ref="F12" r:id="rId31" tooltip="Component" display="'Microchip / Atmel" xr:uid="{7A437100-891F-448E-AEF6-0FC30BD93DCE}"/>
+    <hyperlink ref="G12" r:id="rId32" tooltip="Manufacturer" display="'ATTINY44A-MU" xr:uid="{62137D90-DF69-41BE-9D97-27A0A24BA2E6}"/>
+    <hyperlink ref="I12" r:id="rId33" tooltip="Supplier" display="'ATTINY44A-MU-ND" xr:uid="{C5A28412-2536-4C2E-9CF8-DF2520FE2FF2}"/>
+    <hyperlink ref="F13" r:id="rId34" tooltip="Component" display="'Alpha &amp; Omega Semiconductor" xr:uid="{260F3290-EB30-43E7-BEFA-C34C20AAB777}"/>
+    <hyperlink ref="G13" r:id="rId35" tooltip="Manufacturer" display="'AO3400A" xr:uid="{40B54ED4-B15C-4368-9ABC-21EB47B08808}"/>
+    <hyperlink ref="I13" r:id="rId36" tooltip="Supplier" display="'785-1000-1-ND" xr:uid="{B4070004-2201-493E-B950-F48359D53F80}"/>
+    <hyperlink ref="F14" r:id="rId37" tooltip="Component" display="'Osram Opto" xr:uid="{F56900AA-6760-45BC-B2EF-A1700AB1DF47}"/>
+    <hyperlink ref="G14" r:id="rId38" tooltip="Manufacturer" display="'SFH3015FA" xr:uid="{84268D9F-0135-4D3E-BE0D-4F3F7B60424A}"/>
+    <hyperlink ref="I14" r:id="rId39" tooltip="Supplier" display="'475-2914-1-ND" xr:uid="{5BBE1EFB-4A1C-4721-9557-54CD4B05E9B4}"/>
+    <hyperlink ref="F15" r:id="rId40" tooltip="Component" display="'Bel" xr:uid="{7108B68D-92C7-4F4C-A968-959E308638C9}"/>
+    <hyperlink ref="G15" r:id="rId41" tooltip="Manufacturer" display="'0ZCJ0020FF2E" xr:uid="{0504A96E-4501-41A7-BABB-CDAB52188F2C}"/>
+    <hyperlink ref="I15" r:id="rId42" tooltip="Supplier" display="'507-1797-1-ND" xr:uid="{F9D6FEA5-F355-4A28-8ECC-23F92BA1E74B}"/>
+    <hyperlink ref="F16" r:id="rId43" tooltip="Component" display="'Murata" xr:uid="{41A0384D-33EC-48D1-A511-824137CB4730}"/>
+    <hyperlink ref="G16" r:id="rId44" tooltip="Manufacturer" display="'PRG18BB221MB1RB" xr:uid="{9976366E-A27A-4A74-BC45-79FDCA7FD51D}"/>
+    <hyperlink ref="I16" r:id="rId45" tooltip="Supplier" display="'490-2470-1-ND" xr:uid="{DCE0E737-3643-42DA-81FE-092530FE6242}"/>
+    <hyperlink ref="F17" r:id="rId46" tooltip="Component" display="'Yageo" xr:uid="{E2B6D172-076B-49D9-993C-7FA5B90D97D8}"/>
+    <hyperlink ref="G17" r:id="rId47" tooltip="Manufacturer" display="'RC0603FR-07330RL" xr:uid="{3F3E5866-3E1D-4ED8-A60C-72A9B0D45BAE}"/>
+    <hyperlink ref="I17" r:id="rId48" tooltip="Supplier" display="'311-330HRCT-ND" xr:uid="{99410CA9-DD7F-4EE7-A59F-570DECFDC88E}"/>
+    <hyperlink ref="F18" r:id="rId49" tooltip="Component" display="'Yageo" xr:uid="{68A86FF2-233E-44B4-B8A2-7BE87F6B9ACB}"/>
+    <hyperlink ref="G18" r:id="rId50" tooltip="Manufacturer" display="'RC0603FR-076K8L" xr:uid="{D56B6FD9-5BF7-4E00-A5DD-F94C653AE0CE}"/>
+    <hyperlink ref="I18" r:id="rId51" tooltip="Supplier" display="'311-6.80KHRCT-ND" xr:uid="{48711746-17AB-4B9C-9799-E8FA3D789EF8}"/>
+    <hyperlink ref="F19" r:id="rId52" tooltip="Component" display="'Yageo" xr:uid="{02EAD051-949B-4BD4-BFCF-2F16A942F966}"/>
+    <hyperlink ref="G19" r:id="rId53" tooltip="Manufacturer" display="'RC0603FR-07100RL" xr:uid="{5D46EA2F-A4FD-4ACD-A5D4-F0992BA20508}"/>
+    <hyperlink ref="I19" r:id="rId54" tooltip="Supplier" display="'311-100HRCT-ND" xr:uid="{AEF97E06-898D-4912-9A37-57B53E9813C7}"/>
+    <hyperlink ref="F20" r:id="rId55" tooltip="Component" display="'Yageo" xr:uid="{484E850C-9E5D-46AE-9DFD-D148C3EB5C93}"/>
+    <hyperlink ref="G20" r:id="rId56" tooltip="Manufacturer" display="'RC0603FR-07390RL" xr:uid="{72FD9486-1573-423C-8117-D2309755A50C}"/>
+    <hyperlink ref="I20" r:id="rId57" tooltip="Supplier" display="'311-390HRCT-ND" xr:uid="{87471606-AE4A-4FCA-8430-C65B602E813B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId58"/>

</xml_diff>